<commit_message>
Added Custom Ships. Save/Load is broken
</commit_message>
<xml_diff>
--- a/Other/TimeSheet Calc.xlsx
+++ b/Other/TimeSheet Calc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
   <si>
     <t>Team Meeting: Choose game and brainstormed</t>
   </si>
@@ -199,6 +199,66 @@
   </si>
   <si>
     <t>Time Left</t>
+  </si>
+  <si>
+    <t>Pushing and finished HighScore Unit Test</t>
+  </si>
+  <si>
+    <t>Team Meeting: Beta Planning</t>
+  </si>
+  <si>
+    <t>Working on Difficulty, Levels, and Level Timers</t>
+  </si>
+  <si>
+    <t>Added High Score</t>
+  </si>
+  <si>
+    <t>Finished High Score, Sound, worked on PowerUps, fixed bugs</t>
+  </si>
+  <si>
+    <t>Finished Help Screen</t>
+  </si>
+  <si>
+    <t>Noah and I talked</t>
+  </si>
+  <si>
+    <t>meeting for beta, implemented load formation</t>
+  </si>
+  <si>
+    <t>implemented Tracker AI, ad mines with their loads</t>
+  </si>
+  <si>
+    <t>edited load/save</t>
+  </si>
+  <si>
+    <t>implemented PowerUp class and its load/save</t>
+  </si>
+  <si>
+    <t>implemented powerups in player and editted a few things</t>
+  </si>
+  <si>
+    <t>repaired load/save unit tests</t>
+  </si>
+  <si>
+    <t>meeting, discussed beta</t>
+  </si>
+  <si>
+    <t>made Beta video</t>
+  </si>
+  <si>
+    <t>Meeting about beta</t>
+  </si>
+  <si>
+    <t>Talked with Robert about level design</t>
+  </si>
+  <si>
+    <t>Added death</t>
+  </si>
+  <si>
+    <t>team meeting</t>
+  </si>
+  <si>
+    <t>fixed powerup spawn on load</t>
   </si>
 </sst>
 </file>
@@ -573,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27.55" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -613,7 +673,7 @@
       </c>
       <c r="D3">
         <f>SUM(C:C)</f>
-        <v>1105</v>
+        <v>1860</v>
       </c>
       <c r="F3" s="8">
         <v>43039</v>
@@ -626,7 +686,7 @@
       </c>
       <c r="I3">
         <f>SUM(H:H)</f>
-        <v>1095</v>
+        <v>1250</v>
       </c>
       <c r="K3" s="1">
         <v>43039</v>
@@ -639,7 +699,7 @@
       </c>
       <c r="N3">
         <f>SUM(M:M)</f>
-        <v>927</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
@@ -654,7 +714,7 @@
       </c>
       <c r="D4">
         <f>D3/60</f>
-        <v>18.416666666666668</v>
+        <v>31</v>
       </c>
       <c r="F4" s="9">
         <v>43040</v>
@@ -667,7 +727,7 @@
       </c>
       <c r="I4">
         <f>I3/60</f>
-        <v>18.25</v>
+        <v>20.833333333333332</v>
       </c>
       <c r="K4" s="4">
         <v>43040</v>
@@ -680,7 +740,7 @@
       </c>
       <c r="N4">
         <f>N3/60</f>
-        <v>15.45</v>
+        <v>21.383333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
@@ -762,7 +822,7 @@
       </c>
       <c r="D7">
         <f>50-D4</f>
-        <v>31.583333333333332</v>
+        <v>19</v>
       </c>
       <c r="F7" s="8">
         <v>43042</v>
@@ -775,7 +835,7 @@
       </c>
       <c r="I7">
         <f>50-I4</f>
-        <v>31.75</v>
+        <v>29.166666666666668</v>
       </c>
       <c r="K7" s="1">
         <v>43041</v>
@@ -788,7 +848,7 @@
       </c>
       <c r="N7">
         <f>50-N4</f>
-        <v>34.549999999999997</v>
+        <v>28.616666666666667</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
@@ -1158,6 +1218,15 @@
       <c r="H20" s="6">
         <v>60</v>
       </c>
+      <c r="K20" s="4">
+        <v>43053</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="M20" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="21" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
@@ -1178,8 +1247,26 @@
       <c r="H21" s="3">
         <v>40</v>
       </c>
+      <c r="K21" s="1">
+        <v>43055</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M21" s="3">
+        <v>75</v>
+      </c>
     </row>
     <row r="22" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="4">
+        <v>43052</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="6">
+        <v>25</v>
+      </c>
       <c r="F22" s="9">
         <v>43050</v>
       </c>
@@ -1189,8 +1276,26 @@
       <c r="H22" s="6">
         <v>15</v>
       </c>
+      <c r="K22" s="4">
+        <v>43055</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="M22" s="6">
+        <v>30</v>
+      </c>
     </row>
     <row r="23" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="1">
+        <v>43053</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="3">
+        <v>40</v>
+      </c>
       <c r="F23" s="8">
         <v>43051</v>
       </c>
@@ -1199,6 +1304,162 @@
       </c>
       <c r="H23" s="3">
         <v>10</v>
+      </c>
+      <c r="K23" s="1">
+        <v>43057</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M23" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="4">
+        <v>43055</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="6">
+        <v>180</v>
+      </c>
+      <c r="F24" s="9">
+        <v>43053</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" s="6">
+        <v>40</v>
+      </c>
+      <c r="K24" s="4">
+        <v>43057</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M24" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="1">
+        <v>43056</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="3">
+        <v>60</v>
+      </c>
+      <c r="F25" s="8">
+        <v>43055</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" s="3">
+        <v>5</v>
+      </c>
+      <c r="K25" s="1">
+        <v>43057</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M25" s="3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="4">
+        <v>43057</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="6">
+        <v>330</v>
+      </c>
+      <c r="F26" s="9">
+        <v>43057</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="6">
+        <v>40</v>
+      </c>
+      <c r="K26" s="4">
+        <v>43057</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="M26" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="1">
+        <v>43057</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="3">
+        <v>30</v>
+      </c>
+      <c r="F27" s="8">
+        <v>43057</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H27" s="3">
+        <v>55</v>
+      </c>
+      <c r="K27" s="1">
+        <v>43058</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M27" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="4">
+        <v>43057</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="6">
+        <v>60</v>
+      </c>
+      <c r="F28" s="9">
+        <v>43058</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="1">
+        <v>43058</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="3">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Release and Fixed Sound
</commit_message>
<xml_diff>
--- a/Other/TimeSheet Calc.xlsx
+++ b/Other/TimeSheet Calc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="117">
   <si>
     <t>Team Meeting: Choose game and brainstormed</t>
   </si>
@@ -340,6 +340,36 @@
   </si>
   <si>
     <t>Release Candidate</t>
+  </si>
+  <si>
+    <t>Images, Debugging, and Comments</t>
+  </si>
+  <si>
+    <t>Debugging,Report and Comments</t>
+  </si>
+  <si>
+    <t>Comments and ReadMe</t>
+  </si>
+  <si>
+    <t>Bug fixes, repaired unit tests, added Boss unit tests</t>
+  </si>
+  <si>
+    <t>fixed loading of Speed and invincibility, and loading medium boss state</t>
+  </si>
+  <si>
+    <t>fixed more bugs (hard boss and loading), had brother test for bugs (got mostly complaints), added more unit tests</t>
+  </si>
+  <si>
+    <t>finished up unit tests</t>
+  </si>
+  <si>
+    <t>Wrote comments and labels</t>
+  </si>
+  <si>
+    <t>Headers and comments, made release video</t>
+  </si>
+  <si>
+    <t>Updated serialization design, personal report</t>
   </si>
 </sst>
 </file>
@@ -721,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27.55" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -761,7 +791,7 @@
       </c>
       <c r="D3">
         <f>SUM(C:C)</f>
-        <v>2315</v>
+        <v>2565</v>
       </c>
       <c r="F3" s="8">
         <v>43039</v>
@@ -787,7 +817,7 @@
       </c>
       <c r="N3">
         <f>SUM(M:M)</f>
-        <v>2253</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
@@ -802,7 +832,7 @@
       </c>
       <c r="D4">
         <f>D3/60</f>
-        <v>38.583333333333336</v>
+        <v>42.75</v>
       </c>
       <c r="F4" s="9">
         <v>43040</v>
@@ -828,7 +858,7 @@
       </c>
       <c r="N4">
         <f>N3/60</f>
-        <v>37.549999999999997</v>
+        <v>47.983333333333334</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
@@ -910,7 +940,7 @@
       </c>
       <c r="D7">
         <f>50-D4</f>
-        <v>11.416666666666664</v>
+        <v>7.25</v>
       </c>
       <c r="F7" s="8">
         <v>43042</v>
@@ -936,7 +966,7 @@
       </c>
       <c r="N7">
         <f>50-N4</f>
-        <v>12.450000000000003</v>
+        <v>2.0166666666666657</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
@@ -1664,7 +1694,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <v>43066</v>
       </c>
@@ -1693,7 +1723,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="4">
         <v>43066</v>
       </c>
@@ -1709,7 +1739,7 @@
       <c r="G34" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="H34" s="10">
+      <c r="H34" s="6">
         <v>80</v>
       </c>
       <c r="K34" s="4">
@@ -1722,7 +1752,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1">
         <v>43068</v>
       </c>
@@ -1742,7 +1772,16 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="4">
+        <v>43071</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="6">
+        <v>90</v>
+      </c>
       <c r="K36" s="11" t="s">
         <v>97</v>
       </c>
@@ -1753,7 +1792,16 @@
         <v>199</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="1">
+        <v>43072</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="3">
+        <v>60</v>
+      </c>
       <c r="K37" s="1">
         <v>43066</v>
       </c>
@@ -1764,7 +1812,16 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="4">
+        <v>43073</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="6">
+        <v>90</v>
+      </c>
       <c r="K38" s="4">
         <v>43067</v>
       </c>
@@ -1773,6 +1830,96 @@
       </c>
       <c r="M38" s="6">
         <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="1">
+        <v>43073</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="10">
+        <v>10</v>
+      </c>
+      <c r="K39" s="1">
+        <v>43069</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="M39" s="3">
+        <v>193</v>
+      </c>
+      <c r="N39">
+        <f>60+60+60+13</f>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K40" s="4">
+        <v>43071</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M40" s="6">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K41" s="1">
+        <v>43072</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="M41" s="3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K42" s="4">
+        <v>43072</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="M42" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K43" s="1">
+        <v>43072</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M43" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K44" s="4">
+        <v>43072</v>
+      </c>
+      <c r="L44" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="M44" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="27.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K45" s="1">
+        <v>43073</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="M45" s="3">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>